<commit_message>
Enhance documentation and instructions in Jupyter notebooks
- Added usage instructions and cell status indicators to DataLoader.ipynb for better user guidance.
- Updated the example Tenant ID in 1_TenantAndCommonMaster.ipynb to reflect a more accurate value.
- Changed the description of the boundary code column in 2_BoundarySetup.ipynb to indicate that it is auto-generated.
- Updated the Tenant And Branding Master.xlsx template file.
</commit_message>
<xml_diff>
--- a/utilities/crs_dataloader/templates/Tenant And Branding Master.xlsx
+++ b/utilities/crs_dataloader/templates/Tenant And Branding Master.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salaudeenn/Documents/urban/CCRS/ccrs/test/Citizen-Complaint-Resolution-System/utilities/crs_dataloader/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9447C6CA-B155-6C4D-8F5D-6538CCFC8F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5240C607-12BE-7B49-8230-06D319ABA962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="1" r:id="rId1"/>
     <sheet name="Tenant Info" sheetId="2" r:id="rId2"/>
-    <sheet name="Tenant Branding Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Tenant Branding Deatils" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -245,7 +245,7 @@
     <t>https://en.wikipedia.org/wiki/logo</t>
   </si>
   <si>
-    <t>• Tenant code should be all captial</t>
+    <t>• The tenant code should be all capital letters.</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>